<commit_message>
core functions, post and execute orders finished
</commit_message>
<xml_diff>
--- a/ejercicio comprobación.xlsx
+++ b/ejercicio comprobación.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DParis\OneDrive\ITESO\MySt\LABS\XEMM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf35db895861915d/ITESO/MySt/LABS/XEMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33AF262-C2E2-4A29-BA1F-3D685A710F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D33AF262-C2E2-4A29-BA1F-3D685A710F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{643AC3E9-1311-4405-B687-75980048931E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9F3151A1-8C9B-4FFC-8B16-0461D33FDEC0}"/>
   </bookViews>
@@ -105,11 +105,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;????????_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.00000%"/>
-    <numFmt numFmtId="180" formatCode="0.000000%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;????????_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
+    <numFmt numFmtId="168" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -191,9 +191,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -201,18 +198,21 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0559D77E-98C8-4E2C-BFD9-5BE794AAFEEA}">
-  <dimension ref="A1:S174"/>
+  <dimension ref="A1:T174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,41 +546,41 @@
     <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I1" s="4" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="I3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="O3" s="4" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="O3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,21 +617,22 @@
       <c r="Q4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>56135.9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.66659999999999997</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>56229</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -640,7 +641,7 @@
       <c r="I5" s="2">
         <v>5.42</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>56276</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -649,18 +650,18 @@
       <c r="O5" s="3">
         <v>3.2789999999999999</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>56276.1</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>56139.199999999997</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -669,18 +670,18 @@
       <c r="E6" s="3">
         <v>0.02</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>56231</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.32</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>56142.1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -689,7 +690,7 @@
       <c r="E7" s="2">
         <v>7.2867000000000001E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>56233</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -701,7 +702,7 @@
       <c r="J7" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="8">
         <f>+I5</f>
         <v>5.42</v>
       </c>
@@ -711,16 +712,16 @@
       <c r="P7" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <f>+O5</f>
         <v>3.2789999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1.4530000000000001</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>56143.1</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -729,7 +730,7 @@
       <c r="E8" s="3">
         <v>0.20022000000000001</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>56234</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -741,7 +742,7 @@
       <c r="J8" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f>+K7*J5</f>
         <v>305015.92</v>
       </c>
@@ -751,16 +752,16 @@
       <c r="P8" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <f>+Q7*P5</f>
         <v>184529.33189999999</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4.4400000000000004</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>56150.6</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -769,7 +770,7 @@
       <c r="E9" s="2">
         <v>0.22170000000000001</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>56235</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -782,11 +783,11 @@
         <f>+J8</f>
         <v>FIAT</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <f>+K8*(1-L9)</f>
         <v>305015.8406958608</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>0.0001*0.0026</f>
         <v>2.6E-7</v>
       </c>
@@ -800,11 +801,11 @@
         <f>+P8</f>
         <v>FIAT</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <f>+Q8*(1+R9)</f>
         <v>184529.37987762628</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9" s="13">
         <f>+L9</f>
         <v>2.6E-7</v>
       </c>
@@ -812,11 +813,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>56150.7</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -825,19 +826,19 @@
       <c r="E10" s="3">
         <v>6.9273000000000001E-2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>56236</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>0.2</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>56153</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -846,19 +847,19 @@
       <c r="E11" s="2">
         <v>1.1581999999999999</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>56238</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>56154.7</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -867,19 +868,19 @@
       <c r="E12" s="3">
         <v>0.96450000000000002</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>56239</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>0.1</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>56156.3</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -888,29 +889,29 @@
       <c r="E13" s="2">
         <v>3.56E-2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>56241</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="O13" s="4" t="s">
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="O13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.3</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>56157.2</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -919,7 +920,7 @@
       <c r="E14" s="3">
         <v>0.3654</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>56243</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -943,13 +944,13 @@
       <c r="Q14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>56157.9</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -958,7 +959,7 @@
       <c r="E15" s="2">
         <v>0.59233599999999997</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>56244</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -967,7 +968,7 @@
       <c r="I15" s="2">
         <v>5.42</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <f>+J5*(1-L9)/(1+L19)</f>
         <v>56275.979740642018</v>
       </c>
@@ -977,20 +978,20 @@
       <c r="O15" s="3">
         <v>3.2789999999999999</v>
       </c>
-      <c r="P15" s="5">
+      <c r="P15" s="4">
         <f>+P5*(1+R9)/(1-R19)</f>
         <v>56276.12025939802</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>56159.7</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -999,19 +1000,19 @@
       <c r="E16" s="3">
         <v>1.1311580000000001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>56248</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>0.01</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>56165.2</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1020,7 +1021,7 @@
       <c r="E17" s="2">
         <v>0.41420000000000001</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>56250</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1032,7 +1033,7 @@
       <c r="J17" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="8">
         <f>+I15</f>
         <v>5.42</v>
       </c>
@@ -1042,17 +1043,17 @@
       <c r="P17" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="8">
         <f>+O15</f>
         <v>3.2789999999999999</v>
       </c>
-      <c r="R17" s="8"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0.16400000000000001</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>56167.1</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1061,7 +1062,7 @@
       <c r="E18" s="3">
         <v>2.4509270000000001</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>56251</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1073,7 +1074,7 @@
       <c r="J18" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="8">
         <f>+J15*K17</f>
         <v>305015.81019427971</v>
       </c>
@@ -1083,17 +1084,17 @@
       <c r="P18" t="s">
         <v>11</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="8">
         <f>+P15*Q17</f>
         <v>184529.39833056609</v>
       </c>
-      <c r="R18" s="8"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1.04</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>56171</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1102,7 +1103,7 @@
       <c r="E19" s="2">
         <v>9.9226999999999996E-2</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>56253</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1114,11 +1115,11 @@
       <c r="J19" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="8">
         <f>+K18*(1+L19)</f>
         <v>305015.84069586074</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="12">
         <f>0.0001*0.001</f>
         <v>1.0000000000000001E-7</v>
       </c>
@@ -1131,12 +1132,12 @@
       <c r="P19" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="Q19" s="8">
         <f>+Q18*(1-R19)</f>
         <v>184529.37987762628</v>
       </c>
-      <c r="R19" s="14">
-        <f t="shared" ref="R10:R19" si="0">+L19</f>
+      <c r="R19" s="13">
+        <f t="shared" ref="R19" si="0">+L19</f>
         <v>1.0000000000000001E-7</v>
       </c>
       <c r="S19" t="s">
@@ -1147,7 +1148,7 @@
       <c r="A20" s="3">
         <v>1.284</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>56171.1</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1156,7 +1157,7 @@
       <c r="E20" s="3">
         <v>3.3E-4</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>56255</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1167,7 +1168,7 @@
       <c r="A21" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>56174</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1176,7 +1177,7 @@
       <c r="E21" s="2">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>56256</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1195,7 +1196,7 @@
       <c r="A22" s="3">
         <v>0.72299999999999998</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>56174.7</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1204,7 +1205,7 @@
       <c r="E22" s="3">
         <v>0.59552700000000003</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>56257</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1215,7 +1216,7 @@
       <c r="A23" s="2">
         <v>2.5190000000000001</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>56178.3</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1224,7 +1225,7 @@
       <c r="E23" s="2">
         <v>4.9619000000000003E-2</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>56259</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -1235,7 +1236,7 @@
       <c r="A24" s="3">
         <v>0.45900000000000002</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>56178.400000000001</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1244,13 +1245,13 @@
       <c r="E24" s="3">
         <v>0.168181</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>56261</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="9">
         <v>2.6E-7</v>
       </c>
     </row>
@@ -1258,7 +1259,7 @@
       <c r="A25" s="2">
         <v>1.4730000000000001</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>56178.6</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1267,7 +1268,7 @@
       <c r="E25" s="2">
         <v>9.9229999999999995E-3</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>56262</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -1281,7 +1282,7 @@
       <c r="A26" s="3">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>56179.5</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1290,13 +1291,13 @@
       <c r="E26" s="3">
         <v>2.4810000000000001E-3</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>56263</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="10">
         <v>1E-4</v>
       </c>
     </row>
@@ -1304,7 +1305,7 @@
       <c r="A27" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>56179.9</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1313,13 +1314,13 @@
       <c r="E27" s="2">
         <v>1.9849999999999998E-3</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>56264</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="11">
         <f>+L25*L26</f>
         <v>2.6E-7</v>
       </c>
@@ -1328,7 +1329,7 @@
       <c r="A28" s="3">
         <v>0.88200000000000001</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>56180.5</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1337,7 +1338,7 @@
       <c r="E28" s="3">
         <v>0.42</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>56267</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -1348,7 +1349,7 @@
       <c r="A29" s="2">
         <v>0.124</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>56180.6</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1357,7 +1358,7 @@
       <c r="E29" s="2">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>56268</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -1368,7 +1369,7 @@
       <c r="A30" s="3">
         <v>10</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>56182.8</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -1377,7 +1378,7 @@
       <c r="E30" s="3">
         <v>3.56E-2</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>56273</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -1388,7 +1389,7 @@
       <c r="A31" s="2">
         <v>0.05</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>56185.3</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1397,7 +1398,7 @@
       <c r="E31" s="2">
         <v>0.187329</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>56275</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -1408,7 +1409,7 @@
       <c r="A32" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>56186</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1417,7 +1418,7 @@
       <c r="E32" s="3">
         <v>0.18207300000000001</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>56281</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -1428,7 +1429,7 @@
       <c r="A33" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>56186.7</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1437,7 +1438,7 @@
       <c r="E33" s="2">
         <v>7.4227000000000001E-2</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="4">
         <v>56282</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -1448,7 +1449,7 @@
       <c r="A34" s="3">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>56189.4</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -1457,7 +1458,7 @@
       <c r="E34" s="3">
         <v>5.9343E-2</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>56286</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1468,7 +1469,7 @@
       <c r="A35" s="2">
         <v>4.4450000000000003</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>56189.5</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1477,7 +1478,7 @@
       <c r="E35" s="2">
         <v>0.1903</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <v>56287</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -1488,7 +1489,7 @@
       <c r="A36" s="3">
         <v>1.855</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>56190.5</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1497,7 +1498,7 @@
       <c r="E36" s="3">
         <v>0.01</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>56289</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -1508,7 +1509,7 @@
       <c r="A37" s="2">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>56191.3</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1517,7 +1518,7 @@
       <c r="E37" s="2">
         <v>0.94815899999999997</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>56290</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -1528,7 +1529,7 @@
       <c r="A38" s="3">
         <v>2.5449999999999999</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>56195.4</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1537,7 +1538,7 @@
       <c r="E38" s="3">
         <v>0.1</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>56291</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -1548,7 +1549,7 @@
       <c r="A39" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>56195.5</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1557,7 +1558,7 @@
       <c r="E39" s="2">
         <v>9.7920000000000004E-3</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="4">
         <v>56292</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -1568,7 +1569,7 @@
       <c r="A40" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <v>56195.8</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1577,7 +1578,7 @@
       <c r="E40" s="3">
         <v>2.4483000000000001E-2</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <v>56293</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -1588,7 +1589,7 @@
       <c r="A41" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="4">
         <v>56198.1</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1597,7 +1598,7 @@
       <c r="E41" s="2">
         <v>4.8966000000000003E-2</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="4">
         <v>56295</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -1608,7 +1609,7 @@
       <c r="A42" s="3">
         <v>1E-3</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="5">
         <v>56199.6</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -1617,7 +1618,7 @@
       <c r="E42" s="3">
         <v>0.1</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="5">
         <v>56297</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -1628,7 +1629,7 @@
       <c r="A43" s="2">
         <v>0.35599999999999998</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>56200</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1637,7 +1638,7 @@
       <c r="E43" s="2">
         <v>0.996</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="4">
         <v>56298</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -1648,7 +1649,7 @@
       <c r="A44" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="5">
         <v>56204.4</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -1657,7 +1658,7 @@
       <c r="E44" s="3">
         <v>1.1942999999999999</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="5">
         <v>56300</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -1668,7 +1669,7 @@
       <c r="A45" s="2">
         <v>0.72199999999999998</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="4">
         <v>56207.3</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -1677,7 +1678,7 @@
       <c r="E45" s="2">
         <v>0.29782199999999998</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="4">
         <v>56301</v>
       </c>
       <c r="G45" s="2" t="s">
@@ -1688,7 +1689,7 @@
       <c r="A46" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>56210.1</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -1697,7 +1698,7 @@
       <c r="E46" s="3">
         <v>0.37947900000000001</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="5">
         <v>56302</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -1708,7 +1709,7 @@
       <c r="A47" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <v>56211.4</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1717,7 +1718,7 @@
       <c r="E47" s="2">
         <v>0.55200000000000005</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="4">
         <v>56304</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -1728,7 +1729,7 @@
       <c r="A48" s="3">
         <v>0.17299999999999999</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <v>56212.6</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -1737,7 +1738,7 @@
       <c r="E48" s="3">
         <v>1.4083000000000001</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="5">
         <v>56305</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -1748,7 +1749,7 @@
       <c r="A49" s="2">
         <v>0.34699999999999998</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>56213.1</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -1757,7 +1758,7 @@
       <c r="E49" s="2">
         <v>0.146897</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="4">
         <v>56306</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -1768,7 +1769,7 @@
       <c r="A50" s="3">
         <v>3.556</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="5">
         <v>56214.6</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -1777,7 +1778,7 @@
       <c r="E50" s="3">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="5">
         <v>56307</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -1788,7 +1789,7 @@
       <c r="A51" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>56214.7</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -1797,7 +1798,7 @@
       <c r="E51" s="2">
         <v>1.4093E-2</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="4">
         <v>56308</v>
       </c>
       <c r="G51" s="2" t="s">
@@ -1808,7 +1809,7 @@
       <c r="A52" s="3">
         <v>1.33</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>56215.4</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -1817,7 +1818,7 @@
       <c r="E52" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="5">
         <v>56309</v>
       </c>
       <c r="G52" s="3" t="s">
@@ -1828,7 +1829,7 @@
       <c r="A53" s="2">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="4">
         <v>56218.400000000001</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -1837,7 +1838,7 @@
       <c r="E53" s="2">
         <v>0.97389999999999999</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F53" s="4">
         <v>56310</v>
       </c>
       <c r="G53" s="2" t="s">
@@ -1848,7 +1849,7 @@
       <c r="A54" s="3">
         <v>0.129</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="5">
         <v>56219.8</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -1857,7 +1858,7 @@
       <c r="E54" s="3">
         <v>0.75429999999999997</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="5">
         <v>56311</v>
       </c>
       <c r="G54" s="3" t="s">
@@ -1868,7 +1869,7 @@
       <c r="A55" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="4">
         <v>56221.1</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -1879,7 +1880,7 @@
       <c r="A56" s="3">
         <v>0.98</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="5">
         <v>56223.3</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -1890,7 +1891,7 @@
       <c r="A57" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="4">
         <v>56224.2</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -1901,7 +1902,7 @@
       <c r="A58" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="5">
         <v>56226.8</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -1912,7 +1913,7 @@
       <c r="A59" s="2">
         <v>3.5539999999999998</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="4">
         <v>56227.3</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -1923,7 +1924,7 @@
       <c r="A60" s="3">
         <v>2.7E-2</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="5">
         <v>56227.6</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -1934,7 +1935,7 @@
       <c r="A61" s="2">
         <v>0.37</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>56227.9</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -1945,7 +1946,7 @@
       <c r="A62" s="3">
         <v>0.08</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="5">
         <v>56229.7</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -1956,7 +1957,7 @@
       <c r="A63" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="4">
         <v>56232.2</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -1967,7 +1968,7 @@
       <c r="A64" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="5">
         <v>56232.5</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -1978,7 +1979,7 @@
       <c r="A65" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <v>56233.7</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -1989,7 +1990,7 @@
       <c r="A66" s="3">
         <v>0.10299999999999999</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="5">
         <v>56235.7</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2000,7 +2001,7 @@
       <c r="A67" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="4">
         <v>56235.8</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2011,7 +2012,7 @@
       <c r="A68" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="5">
         <v>56238.2</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2022,7 +2023,7 @@
       <c r="A69" s="2">
         <v>0.27</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="4">
         <v>56241.599999999999</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2033,7 +2034,7 @@
       <c r="A70" s="3">
         <v>1E-3</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="5">
         <v>56243.9</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2044,7 +2045,7 @@
       <c r="A71" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="4">
         <v>56244.3</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2055,7 +2056,7 @@
       <c r="A72" s="3">
         <v>0.17899999999999999</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="5">
         <v>56245.7</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -2066,7 +2067,7 @@
       <c r="A73" s="2">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="4">
         <v>56246.3</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -2077,7 +2078,7 @@
       <c r="A74" s="3">
         <v>4.444</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>56247.6</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -2088,7 +2089,7 @@
       <c r="A75" s="2">
         <v>0.71399999999999997</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="4">
         <v>56248</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -2099,7 +2100,7 @@
       <c r="A76" s="3">
         <v>0.4</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="5">
         <v>56248.1</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -2110,7 +2111,7 @@
       <c r="A77" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="4">
         <v>56254</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -2121,7 +2122,7 @@
       <c r="A78" s="3">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="5">
         <v>56254.5</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -2132,7 +2133,7 @@
       <c r="A79" s="2">
         <v>0.71099999999999997</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="4">
         <v>56256.7</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -2143,7 +2144,7 @@
       <c r="A80" s="3">
         <v>4.444</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="5">
         <v>56257.1</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -2154,7 +2155,7 @@
       <c r="A81" s="2">
         <v>0.25</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="4">
         <v>56260.3</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -2165,7 +2166,7 @@
       <c r="A82" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>56260.6</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -2176,7 +2177,7 @@
       <c r="A83" s="2">
         <v>0.152</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="4">
         <v>56261.4</v>
       </c>
       <c r="C83" s="2" t="s">
@@ -2187,7 +2188,7 @@
       <c r="A84" s="3">
         <v>0.75600000000000001</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <v>56265.1</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -2198,7 +2199,7 @@
       <c r="A85" s="2">
         <v>2.6669999999999998</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="4">
         <v>56266</v>
       </c>
       <c r="C85" s="2" t="s">
@@ -2209,7 +2210,7 @@
       <c r="A86" s="3">
         <v>1.2649999999999999</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>56267.6</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -2220,7 +2221,7 @@
       <c r="A87" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="4">
         <v>56269.7</v>
       </c>
       <c r="C87" s="2" t="s">
@@ -2231,7 +2232,7 @@
       <c r="A88" s="3">
         <v>0.14799999999999999</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="5">
         <v>56270.1</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -2242,7 +2243,7 @@
       <c r="A89" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="4">
         <v>56270.3</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -2253,7 +2254,7 @@
       <c r="A90" s="3">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="5">
         <v>56271.5</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -2264,7 +2265,7 @@
       <c r="A91" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B91" s="4">
         <v>56271.7</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -2275,7 +2276,7 @@
       <c r="A92" s="3">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="5">
         <v>56271.9</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -2286,7 +2287,7 @@
       <c r="A93" s="2">
         <v>5.42</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B93" s="4">
         <v>56276</v>
       </c>
       <c r="C93" s="2" t="s">
@@ -2297,7 +2298,7 @@
       <c r="A94" s="3">
         <v>3.2789999999999999</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="5">
         <v>56276.1</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -2308,7 +2309,7 @@
       <c r="A95" s="2">
         <v>4.444</v>
       </c>
-      <c r="B95" s="5">
+      <c r="B95" s="4">
         <v>56277.2</v>
       </c>
       <c r="C95" s="2" t="s">
@@ -2319,7 +2320,7 @@
       <c r="A96" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="5">
         <v>56283.6</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -2330,7 +2331,7 @@
       <c r="A97" s="2">
         <v>0.443</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B97" s="4">
         <v>56283.7</v>
       </c>
       <c r="C97" s="2" t="s">
@@ -2341,7 +2342,7 @@
       <c r="A98" s="3">
         <v>0.311</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="5">
         <v>56285.599999999999</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -2352,7 +2353,7 @@
       <c r="A99" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="4">
         <v>56289.4</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -2363,7 +2364,7 @@
       <c r="A100" s="3">
         <v>4.444</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="5">
         <v>56290</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -2374,7 +2375,7 @@
       <c r="A101" s="2">
         <v>0.44500000000000001</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B101" s="4">
         <v>56297.2</v>
       </c>
       <c r="C101" s="2" t="s">
@@ -2385,7 +2386,7 @@
       <c r="A102" s="3">
         <v>1.2470000000000001</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="5">
         <v>56298.2</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -2396,7 +2397,7 @@
       <c r="A103" s="2">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B103" s="4">
         <v>56298.6</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -2407,7 +2408,7 @@
       <c r="A104" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="5">
         <v>56299</v>
       </c>
       <c r="C104" s="3" t="s">
@@ -2418,7 +2419,7 @@
       <c r="A105" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="5">
         <v>56300.1</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -2429,7 +2430,7 @@
       <c r="A106" s="3">
         <v>0.71099999999999997</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="5">
         <v>56303.1</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -2440,7 +2441,7 @@
       <c r="A107" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B107" s="4">
         <v>56305.8</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -2451,7 +2452,7 @@
       <c r="A108" s="3">
         <v>2.7E-2</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="5">
         <v>56307.1</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -2462,7 +2463,7 @@
       <c r="A109" s="2">
         <v>0.128</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B109" s="4">
         <v>56310.8</v>
       </c>
       <c r="C109" s="2" t="s">
@@ -2473,7 +2474,7 @@
       <c r="A110" s="3">
         <v>0.56100000000000005</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="5">
         <v>56310.9</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -2484,7 +2485,7 @@
       <c r="A111" s="2">
         <v>0.71399999999999997</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B111" s="4">
         <v>56311</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -2495,7 +2496,7 @@
       <c r="A112" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="5">
         <v>56311.5</v>
       </c>
       <c r="C112" s="3" t="s">
@@ -2506,7 +2507,7 @@
       <c r="A113" s="2">
         <v>2.57</v>
       </c>
-      <c r="B113" s="5">
+      <c r="B113" s="4">
         <v>56311.6</v>
       </c>
       <c r="C113" s="2" t="s">
@@ -2517,7 +2518,7 @@
       <c r="A114" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="5">
         <v>56312.800000000003</v>
       </c>
       <c r="C114" s="3" t="s">
@@ -2528,7 +2529,7 @@
       <c r="A115" s="2">
         <v>1.135</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B115" s="4">
         <v>56314.400000000001</v>
       </c>
       <c r="C115" s="2" t="s">
@@ -2539,7 +2540,7 @@
       <c r="A116" s="3">
         <v>0.15</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="5">
         <v>56314.5</v>
       </c>
       <c r="C116" s="3" t="s">
@@ -2550,7 +2551,7 @@
       <c r="A117" s="2">
         <v>1.637</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B117" s="4">
         <v>56314.7</v>
       </c>
       <c r="C117" s="2" t="s">
@@ -2561,7 +2562,7 @@
       <c r="A118" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="5">
         <v>56315.6</v>
       </c>
       <c r="C118" s="3" t="s">
@@ -2572,7 +2573,7 @@
       <c r="A119" s="2">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B119" s="4">
         <v>56317.599999999999</v>
       </c>
       <c r="C119" s="2" t="s">
@@ -2583,7 +2584,7 @@
       <c r="A120" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="5">
         <v>56318.400000000001</v>
       </c>
       <c r="C120" s="3" t="s">
@@ -2594,7 +2595,7 @@
       <c r="A121" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B121" s="4">
         <v>56318.5</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -2605,7 +2606,7 @@
       <c r="A122" s="3">
         <v>0.25</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="5">
         <v>56319.4</v>
       </c>
       <c r="C122" s="3" t="s">
@@ -2616,7 +2617,7 @@
       <c r="A123" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B123" s="4">
         <v>56319.9</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -2627,7 +2628,7 @@
       <c r="A124" s="3">
         <v>1.8109999999999999</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="5">
         <v>56321.8</v>
       </c>
       <c r="C124" s="3" t="s">
@@ -2638,7 +2639,7 @@
       <c r="A125" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="B125" s="5">
+      <c r="B125" s="4">
         <v>56322.2</v>
       </c>
       <c r="C125" s="2" t="s">
@@ -2649,7 +2650,7 @@
       <c r="A126" s="3">
         <v>0.08</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B126" s="5">
         <v>56323</v>
       </c>
       <c r="C126" s="3" t="s">
@@ -2660,7 +2661,7 @@
       <c r="A127" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="4">
         <v>56324.2</v>
       </c>
       <c r="C127" s="2" t="s">
@@ -2671,7 +2672,7 @@
       <c r="A128" s="3">
         <v>0.03</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="5">
         <v>56328.1</v>
       </c>
       <c r="C128" s="3" t="s">
@@ -2682,7 +2683,7 @@
       <c r="A129" s="2">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B129" s="4">
         <v>56328.2</v>
       </c>
       <c r="C129" s="2" t="s">
@@ -2693,7 +2694,7 @@
       <c r="A130" s="3">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="5">
         <v>56330.9</v>
       </c>
       <c r="C130" s="3" t="s">
@@ -2704,7 +2705,7 @@
       <c r="A131" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131" s="4">
         <v>56331.3</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -2715,7 +2716,7 @@
       <c r="A132" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="5">
         <v>56333.8</v>
       </c>
       <c r="C132" s="3" t="s">
@@ -2726,7 +2727,7 @@
       <c r="A133" s="2">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B133" s="4">
         <v>56334.2</v>
       </c>
       <c r="C133" s="2" t="s">
@@ -2737,7 +2738,7 @@
       <c r="A134" s="3">
         <v>0.5</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="5">
         <v>56336.7</v>
       </c>
       <c r="C134" s="3" t="s">
@@ -2748,7 +2749,7 @@
       <c r="A135" s="2">
         <v>4.4429999999999996</v>
       </c>
-      <c r="B135" s="5">
+      <c r="B135" s="4">
         <v>56339</v>
       </c>
       <c r="C135" s="2" t="s">
@@ -2759,7 +2760,7 @@
       <c r="A136" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="5">
         <v>56339.6</v>
       </c>
       <c r="C136" s="3" t="s">
@@ -2770,7 +2771,7 @@
       <c r="A137" s="2">
         <v>5.5E-2</v>
       </c>
-      <c r="B137" s="5">
+      <c r="B137" s="4">
         <v>56342.5</v>
       </c>
       <c r="C137" s="2" t="s">
@@ -2781,7 +2782,7 @@
       <c r="A138" s="3">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="5">
         <v>56347.1</v>
       </c>
       <c r="C138" s="3" t="s">
@@ -2792,7 +2793,7 @@
       <c r="A139" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B139" s="5">
+      <c r="B139" s="4">
         <v>56350.6</v>
       </c>
       <c r="C139" s="2" t="s">
@@ -2803,7 +2804,7 @@
       <c r="A140" s="3">
         <v>3.5550000000000002</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="5">
         <v>56354.2</v>
       </c>
       <c r="C140" s="3" t="s">
@@ -2814,7 +2815,7 @@
       <c r="A141" s="2">
         <v>10</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B141" s="4">
         <v>56355.1</v>
       </c>
       <c r="C141" s="2" t="s">
@@ -2825,7 +2826,7 @@
       <c r="A142" s="3">
         <v>1.9E-2</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="5">
         <v>56356.4</v>
       </c>
       <c r="C142" s="3" t="s">
@@ -2836,7 +2837,7 @@
       <c r="A143" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143" s="4">
         <v>56358.7</v>
       </c>
       <c r="C143" s="2" t="s">
@@ -2847,7 +2848,7 @@
       <c r="A144" s="3">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="5">
         <v>56362</v>
       </c>
       <c r="C144" s="3" t="s">
@@ -2858,7 +2859,7 @@
       <c r="A145" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B145" s="5">
+      <c r="B145" s="4">
         <v>56362.2</v>
       </c>
       <c r="C145" s="2" t="s">
@@ -2869,7 +2870,7 @@
       <c r="A146" s="3">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="5">
         <v>56362.400000000001</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -2880,7 +2881,7 @@
       <c r="A147" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B147" s="4">
         <v>56363.3</v>
       </c>
       <c r="C147" s="2" t="s">
@@ -2891,7 +2892,7 @@
       <c r="A148" s="3">
         <v>0.47599999999999998</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="5">
         <v>56367.6</v>
       </c>
       <c r="C148" s="3" t="s">
@@ -2902,7 +2903,7 @@
       <c r="A149" s="2">
         <v>4.4429999999999996</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B149" s="4">
         <v>56367.8</v>
       </c>
       <c r="C149" s="2" t="s">
@@ -2913,7 +2914,7 @@
       <c r="A150" s="3">
         <v>0.72</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="5">
         <v>56368.3</v>
       </c>
       <c r="C150" s="3" t="s">
@@ -2924,7 +2925,7 @@
       <c r="A151" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B151" s="4">
         <v>56368.7</v>
       </c>
       <c r="C151" s="2" t="s">
@@ -2935,7 +2936,7 @@
       <c r="A152" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B152" s="6">
+      <c r="B152" s="5">
         <v>56378.9</v>
       </c>
       <c r="C152" s="3" t="s">
@@ -2946,7 +2947,7 @@
       <c r="A153" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="B153" s="5">
+      <c r="B153" s="4">
         <v>56379.9</v>
       </c>
       <c r="C153" s="2" t="s">
@@ -2957,7 +2958,7 @@
       <c r="A154" s="3">
         <v>2E-3</v>
       </c>
-      <c r="B154" s="6">
+      <c r="B154" s="5">
         <v>56384.5</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -2968,7 +2969,7 @@
       <c r="A155" s="2">
         <v>2E-3</v>
       </c>
-      <c r="B155" s="5">
+      <c r="B155" s="4">
         <v>56385.3</v>
       </c>
       <c r="C155" s="2" t="s">
@@ -2979,7 +2980,7 @@
       <c r="A156" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B156" s="6">
+      <c r="B156" s="5">
         <v>56387.5</v>
       </c>
       <c r="C156" s="3" t="s">
@@ -2990,7 +2991,7 @@
       <c r="A157" s="2">
         <v>0.1</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157" s="4">
         <v>56391.199999999997</v>
       </c>
       <c r="C157" s="2" t="s">
@@ -3001,7 +3002,7 @@
       <c r="A158" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="B158" s="6">
+      <c r="B158" s="5">
         <v>56392.2</v>
       </c>
       <c r="C158" s="3" t="s">
@@ -3012,7 +3013,7 @@
       <c r="A159" s="2">
         <v>0.98699999999999999</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159" s="4">
         <v>56392.3</v>
       </c>
       <c r="C159" s="2" t="s">
@@ -3023,7 +3024,7 @@
       <c r="A160" s="3">
         <v>0.2</v>
       </c>
-      <c r="B160" s="6">
+      <c r="B160" s="5">
         <v>56393.7</v>
       </c>
       <c r="C160" s="3" t="s">
@@ -3034,7 +3035,7 @@
       <c r="A161" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B161" s="5">
+      <c r="B161" s="4">
         <v>56394.2</v>
       </c>
       <c r="C161" s="2" t="s">
@@ -3045,7 +3046,7 @@
       <c r="A162" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B162" s="6">
+      <c r="B162" s="5">
         <v>56394.8</v>
       </c>
       <c r="C162" s="3" t="s">
@@ -3056,7 +3057,7 @@
       <c r="A163" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B163" s="5">
+      <c r="B163" s="4">
         <v>56396.3</v>
       </c>
       <c r="C163" s="2" t="s">
@@ -3067,7 +3068,7 @@
       <c r="A164" s="3">
         <v>1E-3</v>
       </c>
-      <c r="B164" s="6">
+      <c r="B164" s="5">
         <v>56398.8</v>
       </c>
       <c r="C164" s="3" t="s">
@@ -3078,7 +3079,7 @@
       <c r="A165" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="B165" s="5">
+      <c r="B165" s="4">
         <v>56400</v>
       </c>
       <c r="C165" s="2" t="s">
@@ -3089,7 +3090,7 @@
       <c r="A166" s="3">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="B166" s="6">
+      <c r="B166" s="5">
         <v>56400.1</v>
       </c>
       <c r="C166" s="3" t="s">
@@ -3100,7 +3101,7 @@
       <c r="A167" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B167" s="5">
+      <c r="B167" s="4">
         <v>56402.400000000001</v>
       </c>
       <c r="C167" s="2" t="s">
@@ -3111,7 +3112,7 @@
       <c r="A168" s="3">
         <v>1E-3</v>
       </c>
-      <c r="B168" s="6">
+      <c r="B168" s="5">
         <v>56403.8</v>
       </c>
       <c r="C168" s="3" t="s">
@@ -3122,7 +3123,7 @@
       <c r="A169" s="2">
         <v>2E-3</v>
       </c>
-      <c r="B169" s="5">
+      <c r="B169" s="4">
         <v>56406.6</v>
       </c>
       <c r="C169" s="2" t="s">
@@ -3133,7 +3134,7 @@
       <c r="A170" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B170" s="6">
+      <c r="B170" s="5">
         <v>56408.1</v>
       </c>
       <c r="C170" s="3" t="s">
@@ -3144,7 +3145,7 @@
       <c r="A171" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="B171" s="5">
+      <c r="B171" s="4">
         <v>56413.8</v>
       </c>
       <c r="C171" s="2" t="s">
@@ -3155,7 +3156,7 @@
       <c r="A172" s="3">
         <v>2.589</v>
       </c>
-      <c r="B172" s="6">
+      <c r="B172" s="5">
         <v>56414.2</v>
       </c>
       <c r="C172" s="3" t="s">
@@ -3166,7 +3167,7 @@
       <c r="A173" s="2">
         <v>4.4370000000000003</v>
       </c>
-      <c r="B173" s="5">
+      <c r="B173" s="4">
         <v>56414.3</v>
       </c>
       <c r="C173" s="2" t="s">
@@ -3177,7 +3178,7 @@
       <c r="A174" s="3">
         <v>2.5299999999999998</v>
       </c>
-      <c r="B174" s="6">
+      <c r="B174" s="5">
         <v>56414.400000000001</v>
       </c>
       <c r="C174" s="3" t="s">
@@ -3186,14 +3187,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O13:Q13"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O13:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>